<commit_message>
Soft code for pruning network.
</commit_message>
<xml_diff>
--- a/Assignment02/testing_class.xlsx
+++ b/Assignment02/testing_class.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,32 +385,32 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -418,10 +418,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -462,10 +462,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -476,10 +476,10 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -487,10 +487,10 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -498,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -517,10 +517,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -539,10 +539,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -550,10 +550,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -572,21 +572,21 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -597,10 +597,10 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -608,10 +608,10 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -627,10 +627,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -638,24 +638,24 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -671,10 +671,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -707,10 +707,10 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -729,10 +729,10 @@
         <v>0</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -754,6 +754,160 @@
         <v>0</v>
       </c>
       <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
         <v>0</v>
       </c>
     </row>

</xml_diff>